<commit_message>
update list of analyses
</commit_message>
<xml_diff>
--- a/static/Analyses_covered/Analyses_viewed_in_class.xlsx
+++ b/static/Analyses_covered/Analyses_viewed_in_class.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmyszkowski/Documents/GitHub/personal-website-2022/static/Analyses_covered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{264106DD-A47C-2D46-852C-70E4A4DD5EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609673B-F63E-C14E-8522-7678E3DA4A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="1900" windowWidth="36000" windowHeight="21580" xr2:uid="{3C13C7B6-1A00-7E46-92D7-E11AFB1CA539}"/>
+    <workbookView xWindow="140" yWindow="1040" windowWidth="25040" windowHeight="21280" xr2:uid="{3C13C7B6-1A00-7E46-92D7-E11AFB1CA539}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="156">
   <si>
     <t>link_youtube_spss</t>
   </si>
@@ -495,6 +494,15 @@
   </si>
   <si>
     <t>One binary DV ~ 1 categorical group IV, Bernouilli/Binomial distributions, odds ratios, model formulation and assumptions, estimation, likelihood ratio tests, Wald tests</t>
+  </si>
+  <si>
+    <t>https://youtu.be/qkbNAihQFck</t>
+  </si>
+  <si>
+    <t>Standard score conversions / z scores / T scores</t>
+  </si>
+  <si>
+    <t>Calculation of different standard scores (z, T, IQ, etc.) from raw scores</t>
   </si>
 </sst>
 </file>
@@ -874,13 +882,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89AA8A63-66C5-3C42-90C3-EA373D3F3F6C}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1680,6 +1688,20 @@
         <v>131</v>
       </c>
     </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" t="s">
+        <v>44</v>
+      </c>
+      <c r="M47" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
Update analyses covered and viewed files
Refreshed HTML widgets in Analyses_covered_in_PHD_Clinical.html and Analyses_viewed_in_doc_programs.html, updated Analyses_viewed_in_class.xlsx, and added a temporary Excel lock file. These changes likely reflect updates to the analyses content or presentation in the referenced files.
</commit_message>
<xml_diff>
--- a/static/Analyses_covered/Analyses_viewed_in_class.xlsx
+++ b/static/Analyses_covered/Analyses_viewed_in_class.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmyszkowski/Documents/GitHub/personal-website-2022/static/Analyses_covered/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609673B-F63E-C14E-8522-7678E3DA4A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F6C530-6E83-B649-B75D-1C009FCC63C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="140" yWindow="1040" windowWidth="25040" windowHeight="21280" xr2:uid="{3C13C7B6-1A00-7E46-92D7-E11AFB1CA539}"/>
   </bookViews>
@@ -352,9 +352,6 @@
     <t>https://youtu.be/8YweDrKsxao</t>
   </si>
   <si>
-    <t>https://youtu.be/sbE6vp3JoEQ</t>
-  </si>
-  <si>
     <t>https://youtu.be/kBl6NIGgDCI</t>
   </si>
   <si>
@@ -503,6 +500,9 @@
   </si>
   <si>
     <t>Calculation of different standard scores (z, T, IQ, etc.) from raw scores</t>
+  </si>
+  <si>
+    <t>https://youtu.be/DuC7cEgM188</t>
   </si>
 </sst>
 </file>
@@ -885,10 +885,10 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C47" sqref="C47"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -908,7 +908,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -923,13 +923,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I1" t="s">
         <v>5</v>
@@ -944,7 +944,7 @@
         <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -964,7 +964,7 @@
         <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1040,7 +1040,7 @@
         <v>101</v>
       </c>
       <c r="M7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1060,27 +1060,27 @@
         <v>103</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="L8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" t="s">
         <v>111</v>
-      </c>
-      <c r="B9" t="s">
-        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>44</v>
       </c>
       <c r="L9" t="s">
+        <v>112</v>
+      </c>
+      <c r="M9" t="s">
         <v>113</v>
-      </c>
-      <c r="M9" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1105,10 +1105,10 @@
         <v>44</v>
       </c>
       <c r="L11" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" t="s">
         <v>124</v>
-      </c>
-      <c r="M11" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1178,7 +1178,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1240,7 +1240,7 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B20" t="s">
         <v>60</v>
@@ -1255,12 +1255,12 @@
         <v>96</v>
       </c>
       <c r="L20" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B21" t="s">
         <v>59</v>
@@ -1272,7 +1272,7 @@
         <v>35</v>
       </c>
       <c r="J21" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
@@ -1306,12 +1306,12 @@
         <v>35</v>
       </c>
       <c r="J23" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
         <v>56</v>
@@ -1340,7 +1340,7 @@
         <v>35</v>
       </c>
       <c r="J25" t="s">
-        <v>105</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
@@ -1388,7 +1388,7 @@
         <v>35</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -1442,13 +1442,13 @@
         <v>91</v>
       </c>
       <c r="J31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="L31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -1465,7 +1465,7 @@
         <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -1473,7 +1473,7 @@
         <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E33" t="s">
         <v>14</v>
@@ -1482,7 +1482,7 @@
         <v>35</v>
       </c>
       <c r="J33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -1502,7 +1502,7 @@
         <v>74</v>
       </c>
       <c r="L34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -1522,7 +1522,7 @@
         <v>74</v>
       </c>
       <c r="K35" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -1541,10 +1541,10 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F37" t="s">
         <v>50</v>
@@ -1553,15 +1553,15 @@
         <v>13</v>
       </c>
       <c r="J37" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F38" t="s">
         <v>50</v>
@@ -1570,12 +1570,12 @@
         <v>13</v>
       </c>
       <c r="J38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B39" t="s">
         <v>78</v>
@@ -1587,15 +1587,15 @@
         <v>13</v>
       </c>
       <c r="J39" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" t="s">
         <v>150</v>
-      </c>
-      <c r="B40" t="s">
-        <v>151</v>
       </c>
       <c r="F40" t="s">
         <v>50</v>
@@ -1604,7 +1604,7 @@
         <v>13</v>
       </c>
       <c r="M40" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -1612,7 +1612,7 @@
         <v>79</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F41" t="s">
         <v>50</v>
@@ -1621,7 +1621,7 @@
         <v>13</v>
       </c>
       <c r="J41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
@@ -1679,27 +1679,27 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>127</v>
+      </c>
+      <c r="B46" t="s">
         <v>128</v>
       </c>
-      <c r="B46" t="s">
-        <v>129</v>
-      </c>
       <c r="J46" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" t="s">
         <v>154</v>
-      </c>
-      <c r="B47" t="s">
-        <v>155</v>
       </c>
       <c r="C47" t="s">
         <v>44</v>
       </c>
       <c r="M47" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>